<commit_message>
Update on Thesis Defense
</commit_message>
<xml_diff>
--- a/Book1 (version 1).xlsx
+++ b/Book1 (version 1).xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Information Systems Engineering\Git Information-Systems-Engineering-UTP\Thesis - Johel H. Batista C\Thesis-UTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96EB9494-0F47-4C70-BEE6-E8F78DC45C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3E7059-A574-4B4D-9A90-C7FA65A0B367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25815" yWindow="0" windowWidth="25890" windowHeight="20985" xr2:uid="{11819DFD-0FC4-4E27-8240-35658D9B665B}"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="30795" windowHeight="20985" activeTab="1" xr2:uid="{11819DFD-0FC4-4E27-8240-35658D9B665B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Estudiantes Emparejados</t>
   </si>
@@ -54,18 +54,68 @@
   <si>
     <t>Estudiantes/Grupo</t>
   </si>
+  <si>
+    <t>Colaborativo</t>
+  </si>
+  <si>
+    <t>Participativo</t>
+  </si>
+  <si>
+    <t>Independiente</t>
+  </si>
+  <si>
+    <t>Competitivo</t>
+  </si>
+  <si>
+    <t>Dependiente</t>
+  </si>
+  <si>
+    <t>Evitativo</t>
+  </si>
+  <si>
+    <t>Experto</t>
+  </si>
+  <si>
+    <t>Autoridad Formal</t>
+  </si>
+  <si>
+    <t>Modelo Personal</t>
+  </si>
+  <si>
+    <t>Facilitador</t>
+  </si>
+  <si>
+    <t>Delegador</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Hanken Grotesk"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Hanken Grotesk"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -84,12 +134,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9E9E9E"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9E9E9E"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9E9E9E"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9E9E9E"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,14 +278,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Tutores</a:t>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Tutores Emparejados | Tamaño de Grupo de Tutoría</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Emparejados según tamaño del grupo de Tutoría</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -311,14 +441,40 @@
             <c:trendlineType val="poly"/>
             <c:order val="6"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.5085714944489916E-3"/>
-                  <c:y val="-0.36689956009019997"/>
+                  <c:x val="1.7581843265199463E-2"/>
+                  <c:y val="5.6171922171700368E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                      <a:t>R² = 0.9988</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -451,9 +607,72 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9398746459767199E-3"/>
+                  <c:y val="-3.9943070496469633E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                      <a:t>R² = 0.9977</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:val>
             <c:numRef>
@@ -619,7 +838,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1</c15:sqref>
@@ -660,7 +879,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$2:$B$11</c15:sqref>
@@ -704,7 +923,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-681C-410B-ADD5-FA82B7AF365E}"/>
                   </c:ext>
@@ -717,7 +936,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$1</c15:sqref>
@@ -758,7 +977,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$2:$C$11</c15:sqref>
@@ -802,7 +1021,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-681C-410B-ADD5-FA82B7AF365E}"/>
                   </c:ext>
@@ -815,7 +1034,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$1</c15:sqref>
@@ -853,7 +1072,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$2:$D$11</c15:sqref>
@@ -867,7 +1086,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-681C-410B-ADD5-FA82B7AF365E}"/>
                   </c:ext>
@@ -880,7 +1099,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$1</c15:sqref>
@@ -918,7 +1137,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$2:$E$11</c15:sqref>
@@ -932,7 +1151,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-681C-410B-ADD5-FA82B7AF365E}"/>
                   </c:ext>
@@ -945,7 +1164,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$1</c15:sqref>
@@ -986,7 +1205,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$2:$F$11</c15:sqref>
@@ -1030,7 +1249,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-681C-410B-ADD5-FA82B7AF365E}"/>
                   </c:ext>
@@ -1160,6 +1379,14 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1248,6 +1475,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Estudiantes Emparejados | Tamaño de Grupo de Tutoría</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1334,14 +1586,46 @@
             <c:trendlineType val="poly"/>
             <c:order val="6"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.9398731408573931E-2"/>
-                  <c:y val="0.3253310002916302"/>
+                  <c:x val="3.0372616598400883E-2"/>
+                  <c:y val="8.4411412306483677E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+                        <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>R² = 0.9989</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400" b="1">
+                      <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1547,6 +1831,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1621,6 +1909,643 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Perfil del</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> Tutor</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Experto</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Autoridad Formal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Modelo Personal</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Facilitador</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Delegador</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-68AF-454A-8236-53EE2397AB64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="496430720"/>
+        <c:axId val="846177696"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="496430720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="846177696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="846177696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="496430720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Perfil del Estudiante</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$4:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Independiente</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Evitativo</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Colaborativo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dependiente</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Competitivo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Participativo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$A$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4D4B-4DFD-89CF-01BF460DE8B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="601753360"/>
+        <c:axId val="842797344"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="601753360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="842797344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="842797344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601753360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2082,7 +3007,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2577,7 +3502,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-464B-4D54-9BE7-D81F75459D82}"/>
                   </c:ext>
@@ -2675,7 +3600,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-464B-4D54-9BE7-D81F75459D82}"/>
                   </c:ext>
@@ -2740,7 +3665,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-464B-4D54-9BE7-D81F75459D82}"/>
                   </c:ext>
@@ -2805,7 +3730,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-464B-4D54-9BE7-D81F75459D82}"/>
                   </c:ext>
@@ -2903,7 +3828,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-464B-4D54-9BE7-D81F75459D82}"/>
                   </c:ext>
@@ -3266,6 +4191,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4273,7 +5278,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4477,22 +5482,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4597,8 +5603,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4730,19 +5736,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4776,7 +5783,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4980,6 +5987,1014 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -5282,23 +7297,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1447799</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>771524</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A58E55BD-16F2-F0AB-3146-DB51F38BFB99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5319,22 +7334,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>261937</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1195387</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{428B258A-0373-3ACA-96FD-6480141ADFDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5359,6 +7374,83 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247055</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>568524</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>172044</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F24221D0-21A3-612E-3B1E-842BDBA21783}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406644</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>113567</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>177311</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A90B570-0A78-8D76-A0FB-EC284AF91A86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -5375,7 +7467,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF962400-A1B4-8F1F-2238-CA8048D39818}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5411,7 +7503,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A58E55BD-16F2-F0AB-3146-DB51F38BFB99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6017,8 +8109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072C9BFB-58FC-4671-900C-26DD32045709}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6359,6 +8451,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E43682-E06A-418D-92E3-A47BBC819CB8}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>3.72</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.29</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C374D8-741D-490C-A9A0-4BA7F23CF084}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update on Thesis Defense Material
</commit_message>
<xml_diff>
--- a/Book1 (version 1).xlsx
+++ b/Book1 (version 1).xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Information Systems Engineering\Git Information-Systems-Engineering-UTP\Thesis - Johel H. Batista C\Thesis-UTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3E7059-A574-4B4D-9A90-C7FA65A0B367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04B056C-9A2F-472A-9526-281554E7E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="30795" windowHeight="20985" activeTab="1" xr2:uid="{11819DFD-0FC4-4E27-8240-35658D9B665B}"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="30795" windowHeight="20985" activeTab="2" xr2:uid="{11819DFD-0FC4-4E27-8240-35658D9B665B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Estudiantes Emparejados</t>
   </si>
@@ -55,19 +55,52 @@
     <t>Estudiantes/Grupo</t>
   </si>
   <si>
+    <t>Nombre del Estudiante</t>
+  </si>
+  <si>
+    <t>Marcelo Hernández</t>
+  </si>
+  <si>
     <t>Colaborativo</t>
+  </si>
+  <si>
+    <t>Sofía Martínez</t>
   </si>
   <si>
     <t>Participativo</t>
   </si>
   <si>
+    <t>Antonio Ruíz</t>
+  </si>
+  <si>
     <t>Independiente</t>
+  </si>
+  <si>
+    <t>Camila Gómez</t>
   </si>
   <si>
     <t>Competitivo</t>
   </si>
   <si>
+    <t>Ricardo Jiménez</t>
+  </si>
+  <si>
     <t>Dependiente</t>
+  </si>
+  <si>
+    <t>Vanessa López</t>
+  </si>
+  <si>
+    <t>Javier Solís</t>
+  </si>
+  <si>
+    <t>Esperanza Reyes</t>
+  </si>
+  <si>
+    <t>Mateo Ortiz</t>
+  </si>
+  <si>
+    <t>Valeria Pérez</t>
   </si>
   <si>
     <t>Evitativo</t>
@@ -87,12 +120,42 @@
   <si>
     <t>Delegador</t>
   </si>
+  <si>
+    <t>Estilo de Aprendizaje</t>
+  </si>
+  <si>
+    <t>Nombre del Tutor</t>
+  </si>
+  <si>
+    <t>Estilo de Enseñanza</t>
+  </si>
+  <si>
+    <t>Óscar Ramírez</t>
+  </si>
+  <si>
+    <t>Patricia González</t>
+  </si>
+  <si>
+    <t>Jorge Mendoza</t>
+  </si>
+  <si>
+    <t>Irene Sandoval</t>
+  </si>
+  <si>
+    <t>Miguel Ángel López</t>
+  </si>
+  <si>
+    <t>Carolina Herrera</t>
+  </si>
+  <si>
+    <t>Ricardo Nuñez</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +177,17 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Hanken Grotesk"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Hanken Grotesk"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Hanken Grotesk"/>
     </font>
@@ -205,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -223,6 +297,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -2545,1492 +2625,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200" b="1">
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Estudiantes Emparejados según Tamaño de Grupo</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Estudiantes Emparejados</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>210</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BBD1-4965-8026-B23A91B6AFAF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="787738911"/>
-        <c:axId val="2065324831"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="787738911"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2065324831"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2065324831"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="787738911"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Tutores Emparejados</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> según Tamaño de Grupo</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!#REF!</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-464B-4D54-9BE7-D81F75459D82}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tutores Emparejados</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$2:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>23</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-464B-4D54-9BE7-D81F75459D82}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1140121487"/>
-        <c:axId val="1131303135"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Estudiantes/Grupo</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$2:$A$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                      <c:pt idx="0">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>10</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-464B-4D54-9BE7-D81F75459D82}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Estudiantes Emparejados</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent2"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$B$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                      <c:pt idx="0">
-                        <c:v>60</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>120</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>169</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>185</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>193</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>201</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>209</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>210</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>210</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>210</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-464B-4D54-9BE7-D81F75459D82}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Estudiantes no Emparejados</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent3"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$2:$C$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                      <c:pt idx="0">
-                        <c:v>150</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>90</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>41</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>25</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-464B-4D54-9BE7-D81F75459D82}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="3"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$D$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent4"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent4"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$D$2:$D$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000005-464B-4D54-9BE7-D81F75459D82}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="4"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent5"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$2:$E$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000006-464B-4D54-9BE7-D81F75459D82}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="5"/>
-                <c:order val="5"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Estudiantes/Grupo</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent6"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$2:$F$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                      <c:pt idx="0">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>10</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000007-464B-4D54-9BE7-D81F75459D82}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1140121487"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1131303135"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1131303135"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1140121487"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="0"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4191,86 +2785,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -6255,1012 +4769,6 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7427,83 +4935,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A90B570-0A78-8D76-A0FB-EC284AF91A86}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7819,292 +5250,6 @@
 </a:theme>
 </file>
 
-<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <a:clrScheme name="Office">
-    <a:dk1>
-      <a:sysClr val="windowText" lastClr="000000"/>
-    </a:dk1>
-    <a:lt1>
-      <a:sysClr val="window" lastClr="FFFFFF"/>
-    </a:lt1>
-    <a:dk2>
-      <a:srgbClr val="44546A"/>
-    </a:dk2>
-    <a:lt2>
-      <a:srgbClr val="E7E6E6"/>
-    </a:lt2>
-    <a:accent1>
-      <a:srgbClr val="4472C4"/>
-    </a:accent1>
-    <a:accent2>
-      <a:srgbClr val="ED7D31"/>
-    </a:accent2>
-    <a:accent3>
-      <a:srgbClr val="A5A5A5"/>
-    </a:accent3>
-    <a:accent4>
-      <a:srgbClr val="FFC000"/>
-    </a:accent4>
-    <a:accent5>
-      <a:srgbClr val="5B9BD5"/>
-    </a:accent5>
-    <a:accent6>
-      <a:srgbClr val="70AD47"/>
-    </a:accent6>
-    <a:hlink>
-      <a:srgbClr val="0563C1"/>
-    </a:hlink>
-    <a:folHlink>
-      <a:srgbClr val="954F72"/>
-    </a:folHlink>
-  </a:clrScheme>
-  <a:fontScheme name="Office">
-    <a:majorFont>
-      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-      <a:ea typeface=""/>
-      <a:cs typeface=""/>
-      <a:font script="Jpan" typeface="游ゴシック Light"/>
-      <a:font script="Hang" typeface="맑은 고딕"/>
-      <a:font script="Hans" typeface="等线 Light"/>
-      <a:font script="Hant" typeface="新細明體"/>
-      <a:font script="Arab" typeface="Times New Roman"/>
-      <a:font script="Hebr" typeface="Times New Roman"/>
-      <a:font script="Thai" typeface="Tahoma"/>
-      <a:font script="Ethi" typeface="Nyala"/>
-      <a:font script="Beng" typeface="Vrinda"/>
-      <a:font script="Gujr" typeface="Shruti"/>
-      <a:font script="Khmr" typeface="MoolBoran"/>
-      <a:font script="Knda" typeface="Tunga"/>
-      <a:font script="Guru" typeface="Raavi"/>
-      <a:font script="Cans" typeface="Euphemia"/>
-      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-      <a:font script="Thaa" typeface="MV Boli"/>
-      <a:font script="Deva" typeface="Mangal"/>
-      <a:font script="Telu" typeface="Gautami"/>
-      <a:font script="Taml" typeface="Latha"/>
-      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-      <a:font script="Orya" typeface="Kalinga"/>
-      <a:font script="Mlym" typeface="Kartika"/>
-      <a:font script="Laoo" typeface="DokChampa"/>
-      <a:font script="Sinh" typeface="Iskoola Pota"/>
-      <a:font script="Mong" typeface="Mongolian Baiti"/>
-      <a:font script="Viet" typeface="Times New Roman"/>
-      <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      <a:font script="Geor" typeface="Sylfaen"/>
-      <a:font script="Armn" typeface="Arial"/>
-      <a:font script="Bugi" typeface="Leelawadee UI"/>
-      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-      <a:font script="Java" typeface="Javanese Text"/>
-      <a:font script="Lisu" typeface="Segoe UI"/>
-      <a:font script="Mymr" typeface="Myanmar Text"/>
-      <a:font script="Nkoo" typeface="Ebrima"/>
-      <a:font script="Olck" typeface="Nirmala UI"/>
-      <a:font script="Osma" typeface="Ebrima"/>
-      <a:font script="Phag" typeface="Phagspa"/>
-      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-      <a:font script="Syre" typeface="Estrangelo Edessa"/>
-      <a:font script="Sora" typeface="Nirmala UI"/>
-      <a:font script="Tale" typeface="Microsoft Tai Le"/>
-      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-      <a:font script="Tfng" typeface="Ebrima"/>
-    </a:majorFont>
-    <a:minorFont>
-      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-      <a:ea typeface=""/>
-      <a:cs typeface=""/>
-      <a:font script="Jpan" typeface="游ゴシック"/>
-      <a:font script="Hang" typeface="맑은 고딕"/>
-      <a:font script="Hans" typeface="等线"/>
-      <a:font script="Hant" typeface="新細明體"/>
-      <a:font script="Arab" typeface="Arial"/>
-      <a:font script="Hebr" typeface="Arial"/>
-      <a:font script="Thai" typeface="Tahoma"/>
-      <a:font script="Ethi" typeface="Nyala"/>
-      <a:font script="Beng" typeface="Vrinda"/>
-      <a:font script="Gujr" typeface="Shruti"/>
-      <a:font script="Khmr" typeface="DaunPenh"/>
-      <a:font script="Knda" typeface="Tunga"/>
-      <a:font script="Guru" typeface="Raavi"/>
-      <a:font script="Cans" typeface="Euphemia"/>
-      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-      <a:font script="Thaa" typeface="MV Boli"/>
-      <a:font script="Deva" typeface="Mangal"/>
-      <a:font script="Telu" typeface="Gautami"/>
-      <a:font script="Taml" typeface="Latha"/>
-      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-      <a:font script="Orya" typeface="Kalinga"/>
-      <a:font script="Mlym" typeface="Kartika"/>
-      <a:font script="Laoo" typeface="DokChampa"/>
-      <a:font script="Sinh" typeface="Iskoola Pota"/>
-      <a:font script="Mong" typeface="Mongolian Baiti"/>
-      <a:font script="Viet" typeface="Arial"/>
-      <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      <a:font script="Geor" typeface="Sylfaen"/>
-      <a:font script="Armn" typeface="Arial"/>
-      <a:font script="Bugi" typeface="Leelawadee UI"/>
-      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-      <a:font script="Java" typeface="Javanese Text"/>
-      <a:font script="Lisu" typeface="Segoe UI"/>
-      <a:font script="Mymr" typeface="Myanmar Text"/>
-      <a:font script="Nkoo" typeface="Ebrima"/>
-      <a:font script="Olck" typeface="Nirmala UI"/>
-      <a:font script="Osma" typeface="Ebrima"/>
-      <a:font script="Phag" typeface="Phagspa"/>
-      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-      <a:font script="Syre" typeface="Estrangelo Edessa"/>
-      <a:font script="Sora" typeface="Nirmala UI"/>
-      <a:font script="Tale" typeface="Microsoft Tai Le"/>
-      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-      <a:font script="Tfng" typeface="Ebrima"/>
-    </a:minorFont>
-  </a:fontScheme>
-  <a:fmtScheme name="Office">
-    <a:fillStyleLst>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:gradFill rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="110000"/>
-              <a:satMod val="105000"/>
-              <a:tint val="67000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="50000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="105000"/>
-              <a:satMod val="103000"/>
-              <a:tint val="73000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="105000"/>
-              <a:satMod val="109000"/>
-              <a:tint val="81000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-      <a:gradFill rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr">
-              <a:satMod val="103000"/>
-              <a:lumMod val="102000"/>
-              <a:tint val="94000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="50000">
-            <a:schemeClr val="phClr">
-              <a:satMod val="110000"/>
-              <a:lumMod val="100000"/>
-              <a:shade val="100000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="99000"/>
-              <a:satMod val="120000"/>
-              <a:shade val="78000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </a:fillStyleLst>
-    <a:lnStyleLst>
-      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="solid"/>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="solid"/>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="solid"/>
-        <a:miter lim="800000"/>
-      </a:ln>
-    </a:lnStyleLst>
-    <a:effectStyleLst>
-      <a:effectStyle>
-        <a:effectLst/>
-      </a:effectStyle>
-      <a:effectStyle>
-        <a:effectLst/>
-      </a:effectStyle>
-      <a:effectStyle>
-        <a:effectLst>
-          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="63000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </a:effectStyle>
-    </a:effectStyleLst>
-    <a:bgFillStyleLst>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:tint val="95000"/>
-          <a:satMod val="170000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:gradFill rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr">
-              <a:tint val="93000"/>
-              <a:satMod val="150000"/>
-              <a:shade val="98000"/>
-              <a:lumMod val="102000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="50000">
-            <a:schemeClr val="phClr">
-              <a:tint val="98000"/>
-              <a:satMod val="130000"/>
-              <a:shade val="90000"/>
-              <a:lumMod val="103000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:shade val="63000"/>
-              <a:satMod val="120000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </a:bgFillStyleLst>
-  </a:fmtScheme>
-</a:themeOverride>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072C9BFB-58FC-4671-900C-26DD32045709}">
   <dimension ref="A1:L11"/>
@@ -8454,27 +5599,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E43682-E06A-418D-92E3-A47BBC819CB8}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I35" sqref="I34:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8496,22 +5641,22 @@
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8541,16 +5686,152 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C374D8-741D-490C-A9A0-4BA7F23CF084}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F34DF9-0275-46C3-87EE-FB017295D2CA}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>